<commit_message>
adding the new test cases
</commit_message>
<xml_diff>
--- a/src/main/java/Windchill/TestDataInput.xlsx
+++ b/src/main/java/Windchill/TestDataInput.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramisetti.nikhila\WindchillBedrock\src\main\java\Windchill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.shrikant.golasangi\WindchillBedrock\src\main\java\Windchill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133FA2CC-88F4-46A4-818C-51FD7E758ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321EEE3A-5B6A-4415-9A83-3A29F67EE4EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Part_Creation" sheetId="2" r:id="rId2"/>
-    <sheet name="ContentFileManagement" sheetId="3" r:id="rId3"/>
-    <sheet name="ReportsManagement" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomActions" sheetId="5" r:id="rId5"/>
+    <sheet name="BaseLine_Creation" sheetId="7" r:id="rId3"/>
+    <sheet name="ContentFileManagement" sheetId="3" r:id="rId4"/>
+    <sheet name="ReportsManagement" sheetId="4" r:id="rId5"/>
+    <sheet name="CustomActions" sheetId="5" r:id="rId6"/>
+    <sheet name="ChangeNotice" sheetId="6" r:id="rId7"/>
+    <sheet name="Product_Creation" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>UserName</t>
   </si>
@@ -170,6 +173,48 @@
   </si>
   <si>
     <t>A.1</t>
+  </si>
+  <si>
+    <t>testuser2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Name_CN</t>
+  </si>
+  <si>
+    <t>Name_CT</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>ChangeNotice_1</t>
+  </si>
+  <si>
+    <t>ChangeTask_1</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>For testing</t>
+  </si>
+  <si>
+    <t>BaseLine 1</t>
+  </si>
+  <si>
+    <t>BaseLine 2</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Testing </t>
   </si>
 </sst>
 </file>
@@ -531,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,6 +609,14 @@
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -651,6 +704,50 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD036CBB-6A9D-46DD-9DE1-FF2302AB5135}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B145A3-871D-4A45-BC1C-7A6AC6914325}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -798,7 +895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632244E-CDBE-4B3A-851C-536A9DB6B732}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -834,7 +931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48DCA-F3E9-4032-8C28-1E2776A80899}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -864,7 +961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -876,6 +973,100 @@
       </c>
       <c r="D2" t="s">
         <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1ACE44-9781-4DFC-90B9-253E7F2ABE90}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01BD39D-E30C-4AA0-861C-6C4AAF94D6FD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/Windchill/TestDataInput.xlsx
+++ b/src/main/java/Windchill/TestDataInput.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramisetti.nikhila\WindchillBedrock\src\main\java\Windchill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.shrikant.golasangi\WindchillBedrock\src\main\java\Windchill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F4AD9D-885A-4299-9752-9A3C9D276E24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24928DCB-AB4D-4B08-A26D-FC0CF9C25853}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Part_Creation" sheetId="2" r:id="rId2"/>
-    <sheet name="ContentFileManagement" sheetId="3" r:id="rId3"/>
-    <sheet name="ReportsManagement" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomActions" sheetId="5" r:id="rId5"/>
+    <sheet name="BaseLine_Creation" sheetId="6" r:id="rId2"/>
+    <sheet name="ChangeNotice" sheetId="7" r:id="rId3"/>
+    <sheet name="Product_Creation" sheetId="8" r:id="rId4"/>
+    <sheet name="Part_Creation" sheetId="2" r:id="rId5"/>
+    <sheet name="ContentFileManagement" sheetId="3" r:id="rId6"/>
+    <sheet name="ReportsManagement" sheetId="4" r:id="rId7"/>
+    <sheet name="CustomActions" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>UserName</t>
   </si>
@@ -170,6 +173,39 @@
   </si>
   <si>
     <t>A.1 (Design)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>BaseLine_1</t>
+  </si>
+  <si>
+    <t>For testing</t>
+  </si>
+  <si>
+    <t>CN_Name</t>
+  </si>
+  <si>
+    <t>CT_Name</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Change_Notice1</t>
+  </si>
+  <si>
+    <t>Change_task1</t>
+  </si>
+  <si>
+    <t>testuser2</t>
+  </si>
+  <si>
+    <t>Product_1</t>
   </si>
 </sst>
 </file>
@@ -531,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +602,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -573,10 +617,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3696481F-B2DA-4AF9-8288-00ED80B40FD9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEFA260-9F02-48F1-B3B1-3D47CACB5C64}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE929234-E2E1-4451-9EE1-676E34E18FDF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1236F5FD-5485-4061-9F51-8033A8C85E37}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B145A3-871D-4A45-BC1C-7A6AC6914325}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -798,7 +963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632244E-CDBE-4B3A-851C-536A9DB6B732}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -834,7 +999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48DCA-F3E9-4032-8C28-1E2776A80899}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Group, CR, PR, ACL Creation
</commit_message>
<xml_diff>
--- a/src/main/java/Windchill/TestDataInput.xlsx
+++ b/src/main/java/Windchill/TestDataInput.xlsx
@@ -5,22 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.shrikant.golasangi\WindchillBedrock\src\main\java\Windchill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramisetti.nikhila\WindchillBedrock\src\main\java\Windchill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24928DCB-AB4D-4B08-A26D-FC0CF9C25853}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003835ED-4DDE-4804-822D-0CCDCE4F0A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="10044" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="BaseLine_Creation" sheetId="6" r:id="rId2"/>
-    <sheet name="ChangeNotice" sheetId="7" r:id="rId3"/>
-    <sheet name="Product_Creation" sheetId="8" r:id="rId4"/>
-    <sheet name="Part_Creation" sheetId="2" r:id="rId5"/>
-    <sheet name="ContentFileManagement" sheetId="3" r:id="rId6"/>
-    <sheet name="ReportsManagement" sheetId="4" r:id="rId7"/>
-    <sheet name="CustomActions" sheetId="5" r:id="rId8"/>
+    <sheet name="GroupCreation" sheetId="9" r:id="rId2"/>
+    <sheet name="SubTypeCreation" sheetId="10" r:id="rId3"/>
+    <sheet name="CRCreation" sheetId="11" r:id="rId4"/>
+    <sheet name="PRCreation" sheetId="12" r:id="rId5"/>
+    <sheet name="ACL_Creation" sheetId="13" r:id="rId6"/>
+    <sheet name="BaseLine_Creation" sheetId="6" r:id="rId7"/>
+    <sheet name="ChangeNotice" sheetId="7" r:id="rId8"/>
+    <sheet name="Product_Creation" sheetId="8" r:id="rId9"/>
+    <sheet name="Part_Creation" sheetId="2" r:id="rId10"/>
+    <sheet name="ContentFileManagement" sheetId="3" r:id="rId11"/>
+    <sheet name="ReportsManagement" sheetId="4" r:id="rId12"/>
+    <sheet name="CustomActions" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>UserName</t>
   </si>
@@ -206,12 +211,114 @@
   </si>
   <si>
     <t>Product_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Members </t>
+  </si>
+  <si>
+    <t>Group Name</t>
+  </si>
+  <si>
+    <t>Object Type Name</t>
+  </si>
+  <si>
+    <t>Subtype name</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>TestDocument</t>
+  </si>
+  <si>
+    <t>TestPart</t>
+  </si>
+  <si>
+    <t>Subtype Display Name</t>
+  </si>
+  <si>
+    <t>To be promoted Stage</t>
+  </si>
+  <si>
+    <t>Sample Part1</t>
+  </si>
+  <si>
+    <t>Promoted to Released stage for Bedrock automation</t>
+  </si>
+  <si>
+    <t>Promoted to cancelled stage for Bedrock automation</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Affected Object Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo CR </t>
+  </si>
+  <si>
+    <t>Change request for bedrock automation testing</t>
+  </si>
+  <si>
+    <t>Test Group</t>
+  </si>
+  <si>
+    <t>Test User1</t>
+  </si>
+  <si>
+    <t>Participant Name</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Deny</t>
+  </si>
+  <si>
+    <t>Test User2</t>
+  </si>
+  <si>
+    <t>wt.part.WTPart</t>
+  </si>
+  <si>
+    <t>Delete,Change Permissions</t>
+  </si>
+  <si>
+    <t>Create,Change Permissions</t>
+  </si>
+  <si>
+    <t>Read,Download</t>
+  </si>
+  <si>
+    <t>wt.doc.WTDocument</t>
+  </si>
+  <si>
+    <t>Modify,Revise</t>
+  </si>
+  <si>
+    <t>Overwrite Permissions</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -277,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -286,6 +393,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,128 +724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3696481F-B2DA-4AF9-8288-00ED80B40FD9}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEFA260-9F02-48F1-B3B1-3D47CACB5C64}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE929234-E2E1-4451-9EE1-676E34E18FDF}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1236F5FD-5485-4061-9F51-8033A8C85E37}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -815,7 +802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B145A3-871D-4A45-BC1C-7A6AC6914325}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -963,7 +950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632244E-CDBE-4B3A-851C-536A9DB6B732}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -999,7 +986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48DCA-F3E9-4032-8C28-1E2776A80899}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1047,4 +1034,415 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A17DE46-8896-4081-B357-19DC209EA4B7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D4AF13-C4C2-4449-9B16-C5FE9F0B7FE7}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC5C15E-4C37-43C4-95D3-52723CFBFCD9}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C1A912-1870-467E-8CD3-7D35949C402D}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34D8971-3518-4779-BB37-B8D743224B45}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3696481F-B2DA-4AF9-8288-00ED80B40FD9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEFA260-9F02-48F1-B3B1-3D47CACB5C64}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE929234-E2E1-4451-9EE1-676E34E18FDF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>